<commit_message>
add lossmodel and run validation
</commit_message>
<xml_diff>
--- a/projects/Kofskey1972_one_stage/Full_Dataset_Kofskey1972_1stage.xlsx
+++ b/projects/Kofskey1972_one_stage/Full_Dataset_Kofskey1972_1stage.xlsx
@@ -461,7 +461,7 @@
         <v>110</v>
       </c>
       <c r="C2" t="n">
-        <v>1.93130817956485</v>
+        <v>2.56469316904405</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +472,7 @@
         <v>90</v>
       </c>
       <c r="C3" t="n">
-        <v>1.94849595800865</v>
+        <v>2.587517790423632</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>1.9416276507849</v>
+        <v>2.578396977491738</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         <v>70</v>
       </c>
       <c r="C5" t="n">
-        <v>1.9769446109482</v>
+        <v>2.625296362810256</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +505,7 @@
         <v>50</v>
       </c>
       <c r="C6" t="n">
-        <v>1.9947671197369</v>
+        <v>2.648963878450305</v>
       </c>
     </row>
     <row r="7">
@@ -516,7 +516,7 @@
         <v>110</v>
       </c>
       <c r="C7" t="n">
-        <v>1.95290310561018</v>
+        <v>2.593370290541536</v>
       </c>
     </row>
     <row r="8">
@@ -527,7 +527,7 @@
         <v>100</v>
       </c>
       <c r="C8" t="n">
-        <v>1.96759764770683</v>
+        <v>2.612884002613113</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +538,7 @@
         <v>90</v>
       </c>
       <c r="C9" t="n">
-        <v>1.97447275908435</v>
+        <v>2.622013851164945</v>
       </c>
     </row>
     <row r="10">
@@ -549,7 +549,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>2.00448685340288</v>
+        <v>2.661871261540083</v>
       </c>
     </row>
     <row r="11">
@@ -560,7 +560,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>2.02077696955951</v>
+        <v>2.683503826488499</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +571,7 @@
         <v>50</v>
       </c>
       <c r="C12" t="n">
-        <v>2.01421825133248</v>
+        <v>2.674794134264062</v>
       </c>
     </row>
     <row r="13">
@@ -582,7 +582,7 @@
         <v>110</v>
       </c>
       <c r="C13" t="n">
-        <v>1.98703419897289</v>
+        <v>2.638694896384126</v>
       </c>
     </row>
     <row r="14">
@@ -593,7 +593,7 @@
         <v>100</v>
       </c>
       <c r="C14" t="n">
-        <v>1.99297859931634</v>
+        <v>2.646588801207925</v>
       </c>
     </row>
     <row r="15">
@@ -604,7 +604,7 @@
         <v>90</v>
       </c>
       <c r="C15" t="n">
-        <v>2.00361154762097</v>
+        <v>2.660708893574452</v>
       </c>
     </row>
     <row r="16">
@@ -615,7 +615,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>2.01955902603398</v>
+        <v>2.681886450518543</v>
       </c>
     </row>
     <row r="17">
@@ -626,7 +626,7 @@
         <v>50</v>
       </c>
       <c r="C17" t="n">
-        <v>2.03365091451066</v>
+        <v>2.700599864823666</v>
       </c>
     </row>
     <row r="18">
@@ -637,7 +637,7 @@
         <v>110</v>
       </c>
       <c r="C18" t="n">
-        <v>1.9995936948175</v>
+        <v>2.655373359997617</v>
       </c>
     </row>
     <row r="19">
@@ -648,7 +648,7 @@
         <v>100</v>
       </c>
       <c r="C19" t="n">
-        <v>2.00335153174461</v>
+        <v>2.66036360381231</v>
       </c>
     </row>
     <row r="20">
@@ -659,7 +659,7 @@
         <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>2.0152286681679</v>
+        <v>2.676135923825722</v>
       </c>
     </row>
     <row r="21">
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
       <c r="C21" t="n">
-        <v>2.04024656957247</v>
+        <v>2.709358607556381</v>
       </c>
     </row>
     <row r="22">
@@ -681,7 +681,7 @@
         <v>50</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0334151991835</v>
+        <v>2.700286845132764</v>
       </c>
     </row>
     <row r="23">
@@ -692,7 +692,7 @@
         <v>110</v>
       </c>
       <c r="C23" t="n">
-        <v>2.01154081682246</v>
+        <v>2.671238617816159</v>
       </c>
     </row>
     <row r="24">
@@ -703,7 +703,7 @@
         <v>110</v>
       </c>
       <c r="C24" t="n">
-        <v>2.00341762923842</v>
+        <v>2.660451378406059</v>
       </c>
     </row>
     <row r="25">
@@ -714,7 +714,7 @@
         <v>100</v>
       </c>
       <c r="C25" t="n">
-        <v>2.00874285158844</v>
+        <v>2.667523041814959</v>
       </c>
     </row>
     <row r="26">
@@ -725,7 +725,7 @@
         <v>90</v>
       </c>
       <c r="C26" t="n">
-        <v>2.02343739368509</v>
+        <v>2.687036753886535</v>
       </c>
     </row>
     <row r="27">
@@ -736,7 +736,7 @@
         <v>30</v>
       </c>
       <c r="C27" t="n">
-        <v>2.04032919143972</v>
+        <v>2.709468325798551</v>
       </c>
     </row>
     <row r="28">
@@ -747,7 +747,7 @@
         <v>70</v>
       </c>
       <c r="C28" t="n">
-        <v>2.03002138448328</v>
+        <v>2.695780006985049</v>
       </c>
     </row>
     <row r="29">
@@ -758,7 +758,7 @@
         <v>110</v>
       </c>
       <c r="C29" t="n">
-        <v>2.00411068090138</v>
+        <v>2.661371720837472</v>
       </c>
     </row>
     <row r="30">
@@ -769,7 +769,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="n">
-        <v>2.03100069661574</v>
+        <v>2.697080490855546</v>
       </c>
     </row>
     <row r="31">
@@ -780,7 +780,7 @@
         <v>100</v>
       </c>
       <c r="C31" t="n">
-        <v>2.01694185688596</v>
+        <v>2.67841096384729</v>
       </c>
     </row>
     <row r="32">
@@ -791,7 +791,7 @@
         <v>90</v>
       </c>
       <c r="C32" t="n">
-        <v>2.02570171885884</v>
+        <v>2.690043679123562</v>
       </c>
     </row>
     <row r="33">
@@ -802,7 +802,7 @@
         <v>70</v>
       </c>
       <c r="C33" t="n">
-        <v>2.02885495812205</v>
+        <v>2.694231043566113</v>
       </c>
     </row>
     <row r="34">
@@ -813,7 +813,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="n">
-        <v>2.04356505257018</v>
+        <v>2.71376540848327</v>
       </c>
     </row>
     <row r="35">
@@ -824,7 +824,7 @@
         <v>50</v>
       </c>
       <c r="C35" t="n">
-        <v>2.03765564501757</v>
+        <v>2.705917972562044</v>
       </c>
     </row>
     <row r="36">
@@ -835,7 +835,7 @@
         <v>110</v>
       </c>
       <c r="C36" t="n">
-        <v>2.00205534045069</v>
+        <v>2.658642318213012</v>
       </c>
     </row>
     <row r="37">
@@ -846,7 +846,7 @@
         <v>100</v>
       </c>
       <c r="C37" t="n">
-        <v>2.01301148605958</v>
+        <v>2.673191602526872</v>
       </c>
     </row>
     <row r="38">
@@ -857,7 +857,7 @@
         <v>90</v>
       </c>
       <c r="C38" t="n">
-        <v>2.01801545514928</v>
+        <v>2.679836655594142</v>
       </c>
     </row>
     <row r="39">
@@ -868,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="C39" t="n">
-        <v>2.04367780711844</v>
+        <v>2.713915141613778</v>
       </c>
     </row>
     <row r="40">
@@ -879,7 +879,7 @@
         <v>70</v>
       </c>
       <c r="C40" t="n">
-        <v>2.03526058288917</v>
+        <v>2.702737434341816</v>
       </c>
     </row>
     <row r="41">
@@ -890,7 +890,7 @@
         <v>110</v>
       </c>
       <c r="C41" t="n">
-        <v>2.00595800865099</v>
+        <v>2.663824891652229</v>
       </c>
     </row>
     <row r="42">
@@ -901,7 +901,7 @@
         <v>50</v>
       </c>
       <c r="C42" t="n">
-        <v>2.03564987768723</v>
+        <v>2.703254400882886</v>
       </c>
     </row>
     <row r="43">
@@ -912,7 +912,7 @@
         <v>100</v>
       </c>
       <c r="C43" t="n">
-        <v>2.0200460090398</v>
+        <v>2.682533142745958</v>
       </c>
     </row>
     <row r="44">
@@ -923,7 +923,7 @@
         <v>30</v>
       </c>
       <c r="C44" t="n">
-        <v>2.04818312893871</v>
+        <v>2.719898012819447</v>
       </c>
     </row>
     <row r="45">
@@ -934,7 +934,7 @@
         <v>90</v>
       </c>
       <c r="C45" t="n">
-        <v>2.01976072059228</v>
+        <v>2.682154292109739</v>
       </c>
     </row>
     <row r="46">
@@ -945,7 +945,7 @@
         <v>70</v>
       </c>
       <c r="C46" t="n">
-        <v>2.02981239976023</v>
+        <v>2.695502484372495</v>
       </c>
     </row>
     <row r="47">
@@ -956,7 +956,7 @@
         <v>50</v>
       </c>
       <c r="C47" t="n">
-        <v>2.04234662303368</v>
+        <v>2.712147387111908</v>
       </c>
     </row>
     <row r="48">
@@ -967,7 +967,7 @@
         <v>110</v>
       </c>
       <c r="C48" t="n">
-        <v>2.01112819349717</v>
+        <v>2.670690672006704</v>
       </c>
     </row>
     <row r="49">
@@ -978,7 +978,7 @@
         <v>100</v>
       </c>
       <c r="C49" t="n">
-        <v>2.00584185202585</v>
+        <v>2.663670640711759</v>
       </c>
     </row>
     <row r="50">
@@ -989,7 +989,7 @@
         <v>90</v>
       </c>
       <c r="C50" t="n">
-        <v>2.02430395126929</v>
+        <v>2.688187504626524</v>
       </c>
     </row>
     <row r="51">
@@ -1000,7 +1000,7 @@
         <v>100</v>
       </c>
       <c r="C51" t="n">
-        <v>2.01587700682035</v>
+        <v>2.676996889326081</v>
       </c>
     </row>
     <row r="52">
@@ -1011,7 +1011,7 @@
         <v>70</v>
       </c>
       <c r="C52" t="n">
-        <v>2.03372576020218</v>
+        <v>2.700699256643059</v>
       </c>
     </row>
     <row r="53">
@@ -1022,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="C53" t="n">
-        <v>2.04156074327279</v>
+        <v>2.711103773008384</v>
       </c>
     </row>
     <row r="54">
@@ -1033,7 +1033,7 @@
         <v>30</v>
       </c>
       <c r="C54" t="n">
-        <v>2.0406397524584</v>
+        <v>2.709880737308846</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1080,7 @@
         <v>110</v>
       </c>
       <c r="C2" t="n">
-        <v>40.9413071653397</v>
+        <v>55.77394263392773</v>
       </c>
     </row>
     <row r="3">
@@ -1091,7 +1091,7 @@
         <v>90</v>
       </c>
       <c r="C3" t="n">
-        <v>50.0090723940011</v>
+        <v>68.1268705861022</v>
       </c>
     </row>
     <row r="4">
@@ -1102,7 +1102,7 @@
         <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>46.1512682836511</v>
+        <v>62.87142174870535</v>
       </c>
     </row>
     <row r="5">
@@ -1113,7 +1113,7 @@
         <v>70</v>
       </c>
       <c r="C5" t="n">
-        <v>61.1031290501759</v>
+        <v>83.24019554713006</v>
       </c>
     </row>
     <row r="6">
@@ -1124,7 +1124,7 @@
         <v>70</v>
       </c>
       <c r="C6" t="n">
-        <v>61.489353823366</v>
+        <v>83.76634578109091</v>
       </c>
     </row>
     <row r="7">
@@ -1135,7 +1135,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>72.48861321977409</v>
+        <v>98.75052936158761</v>
       </c>
     </row>
     <row r="8">
@@ -1146,7 +1146,7 @@
         <v>110</v>
       </c>
       <c r="C8" t="n">
-        <v>45.1905202740233</v>
+        <v>61.56260412453322</v>
       </c>
     </row>
     <row r="9">
@@ -1157,7 +1157,7 @@
         <v>100</v>
       </c>
       <c r="C9" t="n">
-        <v>50.4002962414367</v>
+        <v>68.65983101005197</v>
       </c>
     </row>
     <row r="10">
@@ -1168,7 +1168,7 @@
         <v>90</v>
       </c>
       <c r="C10" t="n">
-        <v>55.3203110535086</v>
+        <v>75.36231910547075</v>
       </c>
     </row>
     <row r="11">
@@ -1179,7 +1179,7 @@
         <v>90</v>
       </c>
       <c r="C11" t="n">
-        <v>55.6102573597482</v>
+        <v>75.75731012482974</v>
       </c>
     </row>
     <row r="12">
@@ -1190,7 +1190,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>84.8400296241436</v>
+        <v>115.5767432194651</v>
       </c>
     </row>
     <row r="13">
@@ -1201,7 +1201,7 @@
         <v>70</v>
       </c>
       <c r="C13" t="n">
-        <v>66.897981855212</v>
+        <v>91.13446689061456</v>
       </c>
     </row>
     <row r="14">
@@ -1212,7 +1212,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>77.3192001481207</v>
+        <v>105.3311907249818</v>
       </c>
     </row>
     <row r="15">
@@ -1223,7 +1223,7 @@
         <v>110</v>
       </c>
       <c r="C15" t="n">
-        <v>51.3743751157193</v>
+        <v>69.98680914086144</v>
       </c>
     </row>
     <row r="16">
@@ -1234,7 +1234,7 @@
         <v>110</v>
       </c>
       <c r="C16" t="n">
-        <v>51.9531568228106</v>
+        <v>70.77527780402629</v>
       </c>
     </row>
     <row r="17">
@@ -1245,7 +1245,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="n">
-        <v>89.47731901499721</v>
+        <v>121.8940772366201</v>
       </c>
     </row>
     <row r="18">
@@ -1256,7 +1256,7 @@
         <v>100</v>
       </c>
       <c r="C18" t="n">
-        <v>56.8739122384743</v>
+        <v>77.47877481648028</v>
       </c>
     </row>
     <row r="19">
@@ -1267,7 +1267,7 @@
         <v>100</v>
       </c>
       <c r="C19" t="n">
-        <v>58.0316608035549</v>
+        <v>79.05596437206887</v>
       </c>
     </row>
     <row r="20">
@@ -1278,7 +1278,7 @@
         <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>62.7591186817256</v>
+        <v>85.49613403828364</v>
       </c>
     </row>
     <row r="21">
@@ -1289,7 +1289,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="n">
-        <v>73.9513053138307</v>
+        <v>100.7431405065018</v>
       </c>
     </row>
     <row r="22">
@@ -1300,7 +1300,7 @@
         <v>50</v>
       </c>
       <c r="C22" t="n">
-        <v>84.6622847620811</v>
+        <v>115.3346031309693</v>
       </c>
     </row>
     <row r="23">
@@ -1311,7 +1311,7 @@
         <v>110</v>
       </c>
       <c r="C23" t="n">
-        <v>56.1103499351971</v>
+        <v>76.43858135298322</v>
       </c>
     </row>
     <row r="24">
@@ -1322,7 +1322,7 @@
         <v>100</v>
       </c>
       <c r="C24" t="n">
-        <v>62.1890390668394</v>
+        <v>84.71952015028467</v>
       </c>
     </row>
     <row r="25">
@@ -1333,7 +1333,7 @@
         <v>90</v>
       </c>
       <c r="C25" t="n">
-        <v>67.3982595815589</v>
+        <v>91.81599034802694</v>
       </c>
     </row>
     <row r="26">
@@ -1344,7 +1344,7 @@
         <v>70</v>
       </c>
       <c r="C26" t="n">
-        <v>78.0122199592668</v>
+        <v>106.275284840857</v>
       </c>
     </row>
     <row r="27">
@@ -1355,7 +1355,7 @@
         <v>30</v>
       </c>
       <c r="C27" t="n">
-        <v>96.05091649694501</v>
+        <v>130.8492248428274</v>
       </c>
     </row>
     <row r="28">
@@ -1366,7 +1366,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="n">
-        <v>96.91927420847991</v>
+        <v>132.0321800668334</v>
       </c>
     </row>
     <row r="29">
@@ -1377,7 +1377,7 @@
         <v>50</v>
       </c>
       <c r="C29" t="n">
-        <v>89.5939640807258</v>
+        <v>122.0529816696956</v>
       </c>
     </row>
     <row r="30">
@@ -1388,7 +1388,7 @@
         <v>110</v>
       </c>
       <c r="C30" t="n">
-        <v>60.8485465654508</v>
+        <v>82.89338031621136</v>
       </c>
     </row>
     <row r="31">
@@ -1399,7 +1399,7 @@
         <v>100</v>
       </c>
       <c r="C31" t="n">
-        <v>65.8659507498611</v>
+        <v>89.72854100178512</v>
       </c>
     </row>
     <row r="32">
@@ -1410,7 +1410,7 @@
         <v>100</v>
       </c>
       <c r="C32" t="n">
-        <v>66.63765969264951</v>
+        <v>90.77983255267159</v>
       </c>
     </row>
     <row r="33">
@@ -1421,7 +1421,7 @@
         <v>90</v>
       </c>
       <c r="C33" t="n">
-        <v>71.36567302351411</v>
+        <v>97.22075890666285</v>
       </c>
     </row>
     <row r="34">
@@ -1432,7 +1432,7 @@
         <v>90</v>
       </c>
       <c r="C34" t="n">
-        <v>72.1373819663025</v>
+        <v>98.27205045754931</v>
       </c>
     </row>
     <row r="35">
@@ -1443,7 +1443,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="n">
-        <v>82.75171264580629</v>
+        <v>112.731849408897</v>
       </c>
     </row>
     <row r="36">
@@ -1454,7 +1454,7 @@
         <v>30</v>
       </c>
       <c r="C36" t="n">
-        <v>100.693945565636</v>
+        <v>137.1743779670066</v>
       </c>
     </row>
     <row r="37">
@@ -1465,7 +1465,7 @@
         <v>110</v>
       </c>
       <c r="C37" t="n">
-        <v>64.81410849842619</v>
+        <v>88.29562658225879</v>
       </c>
     </row>
     <row r="38">
@@ -1476,7 +1476,7 @@
         <v>50</v>
       </c>
       <c r="C38" t="n">
-        <v>92.8855767450472</v>
+        <v>126.5371134335293</v>
       </c>
     </row>
     <row r="39">
@@ -1487,7 +1487,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="n">
-        <v>93.27272727272729</v>
+        <v>127.0645248137845</v>
       </c>
     </row>
     <row r="40">
@@ -1498,7 +1498,7 @@
         <v>100</v>
       </c>
       <c r="C40" t="n">
-        <v>69.54360303647471</v>
+        <v>94.73857077032093</v>
       </c>
     </row>
     <row r="41">
@@ -1509,7 +1509,7 @@
         <v>100</v>
       </c>
       <c r="C41" t="n">
-        <v>69.9297352342159</v>
+        <v>95.26459488965246</v>
       </c>
     </row>
     <row r="42">
@@ -1520,7 +1520,7 @@
         <v>90</v>
       </c>
       <c r="C42" t="n">
-        <v>75.5261988520644</v>
+        <v>102.8886025822792</v>
       </c>
     </row>
     <row r="43">
@@ -1531,7 +1531,7 @@
         <v>70</v>
       </c>
       <c r="C43" t="n">
-        <v>86.04462136641359</v>
+        <v>117.2177467775427</v>
       </c>
     </row>
     <row r="44">
@@ -1542,7 +1542,7 @@
         <v>30</v>
       </c>
       <c r="C44" t="n">
-        <v>104.859100166635</v>
+        <v>142.8485273740931</v>
       </c>
     </row>
     <row r="45">
@@ -1553,7 +1553,7 @@
         <v>30</v>
       </c>
       <c r="C45" t="n">
-        <v>105.823921496019</v>
+        <v>144.1628940419607</v>
       </c>
     </row>
     <row r="46">
@@ -1564,7 +1564,7 @@
         <v>50</v>
       </c>
       <c r="C46" t="n">
-        <v>95.8894649139048</v>
+        <v>130.6292809291102</v>
       </c>
     </row>
     <row r="47">
@@ -1575,7 +1575,7 @@
         <v>50</v>
       </c>
       <c r="C47" t="n">
-        <v>96.4700981299759</v>
+        <v>131.4202718848635</v>
       </c>
     </row>
     <row r="48">
@@ -1586,7 +1586,7 @@
         <v>110</v>
       </c>
       <c r="C48" t="n">
-        <v>68.5963710423995</v>
+        <v>93.44816588204473</v>
       </c>
     </row>
     <row r="49">
@@ -1597,7 +1597,7 @@
         <v>110</v>
       </c>
       <c r="C49" t="n">
-        <v>69.2718015182373</v>
+        <v>94.36829821832919</v>
       </c>
     </row>
     <row r="50">
@@ -1608,7 +1608,7 @@
         <v>100</v>
       </c>
       <c r="C50" t="n">
-        <v>74.38715052768001</v>
+        <v>101.3368881818346</v>
       </c>
     </row>
     <row r="51">
@@ -1619,7 +1619,7 @@
         <v>90</v>
       </c>
       <c r="C51" t="n">
-        <v>79.69376041473799</v>
+        <v>108.5660309697319</v>
       </c>
     </row>
     <row r="52">
@@ -1630,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="C52" t="n">
-        <v>108.252360673949</v>
+        <v>147.4711330010362</v>
       </c>
     </row>
     <row r="53">
@@ -1641,7 +1641,7 @@
         <v>70</v>
       </c>
       <c r="C53" t="n">
-        <v>90.1203480836882</v>
+        <v>122.7700694526058</v>
       </c>
     </row>
     <row r="54">
@@ -1652,7 +1652,7 @@
         <v>50</v>
       </c>
       <c r="C54" t="n">
-        <v>100.645621181262</v>
+        <v>137.1085461304458</v>
       </c>
     </row>
     <row r="55">
@@ -1663,7 +1663,7 @@
         <v>110</v>
       </c>
       <c r="C55" t="n">
-        <v>72.285687835586</v>
+        <v>98.47408609388815</v>
       </c>
     </row>
     <row r="56">
@@ -1674,7 +1674,7 @@
         <v>50</v>
       </c>
       <c r="C56" t="n">
-        <v>101.129235326791</v>
+        <v>137.7673689545623</v>
       </c>
     </row>
     <row r="57">
@@ -1685,7 +1685,7 @@
         <v>100</v>
       </c>
       <c r="C57" t="n">
-        <v>77.3045732271801</v>
+        <v>105.3112646135326</v>
       </c>
     </row>
     <row r="58">
@@ -1696,7 +1696,7 @@
         <v>30</v>
       </c>
       <c r="C58" t="n">
-        <v>111.260877615256</v>
+        <v>151.5696062280882</v>
       </c>
     </row>
     <row r="59">
@@ -1707,7 +1707,7 @@
         <v>100</v>
       </c>
       <c r="C59" t="n">
-        <v>77.8848361414553</v>
+        <v>106.1017511107683</v>
       </c>
     </row>
     <row r="60">
@@ -1718,7 +1718,7 @@
         <v>30</v>
       </c>
       <c r="C60" t="n">
-        <v>110.586928346602</v>
+        <v>150.6514917258744</v>
       </c>
     </row>
     <row r="61">
@@ -1729,7 +1729,7 @@
         <v>90</v>
       </c>
       <c r="C61" t="n">
-        <v>82.42232919829659</v>
+        <v>112.2831335574031</v>
       </c>
     </row>
     <row r="62">
@@ -1740,7 +1740,7 @@
         <v>90</v>
       </c>
       <c r="C62" t="n">
-        <v>83.19422329198289</v>
+        <v>113.3346773375483</v>
       </c>
     </row>
     <row r="63">
@@ -1751,7 +1751,7 @@
         <v>70</v>
       </c>
       <c r="C63" t="n">
-        <v>92.9450101832994</v>
+        <v>126.6180790256201</v>
       </c>
     </row>
     <row r="64">
@@ -1762,7 +1762,7 @@
         <v>50</v>
       </c>
       <c r="C64" t="n">
-        <v>102.209775967413</v>
+        <v>139.2393789092102</v>
       </c>
     </row>
     <row r="65">
@@ -1773,7 +1773,7 @@
         <v>30</v>
       </c>
       <c r="C65" t="n">
-        <v>112.823921496019</v>
+        <v>153.6989256312993</v>
       </c>
     </row>
     <row r="66">
@@ -1784,7 +1784,7 @@
         <v>30</v>
       </c>
       <c r="C66" t="n">
-        <v>113.402888354008</v>
+        <v>154.4876465237226</v>
       </c>
     </row>
     <row r="67">
@@ -1795,7 +1795,7 @@
         <v>110</v>
       </c>
       <c r="C67" t="n">
-        <v>74.2412516200703</v>
+        <v>101.1381315258608</v>
       </c>
     </row>
     <row r="68">
@@ -1806,7 +1806,7 @@
         <v>100</v>
       </c>
       <c r="C68" t="n">
-        <v>79.64691723754861</v>
+        <v>108.5022169672429</v>
       </c>
     </row>
     <row r="69">
@@ -1817,7 +1817,7 @@
         <v>90</v>
       </c>
       <c r="C69" t="n">
-        <v>84.4730605443436</v>
+        <v>115.0768248284246</v>
       </c>
     </row>
     <row r="70">
@@ -1828,7 +1828,7 @@
         <v>90</v>
       </c>
       <c r="C70" t="n">
-        <v>84.4754675060174</v>
+        <v>115.0801038087897</v>
       </c>
     </row>
     <row r="71">
@@ -1839,7 +1839,7 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>94.5130531383077</v>
+        <v>128.75420861882</v>
       </c>
     </row>
     <row r="72">
@@ -1850,7 +1850,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="n">
-        <v>94.5136085910016</v>
+        <v>128.7549653065965</v>
       </c>
     </row>
     <row r="73">
@@ -1861,7 +1861,7 @@
         <v>50</v>
       </c>
       <c r="C73" t="n">
-        <v>103.680429550083</v>
+        <v>141.2428359122552</v>
       </c>
     </row>
     <row r="74">
@@ -1872,7 +1872,7 @@
         <v>30</v>
       </c>
       <c r="C74" t="n">
-        <v>114.873912238474</v>
+        <v>156.4916079852854</v>
       </c>
     </row>
   </sheetData>
@@ -1941,7 +1941,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="n">
-        <v>85.31187486156722</v>
+        <v>85.31187486156723</v>
       </c>
     </row>
     <row r="5">
@@ -1952,7 +1952,7 @@
         <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>84.10389791141228</v>
+        <v>84.10389791141229</v>
       </c>
     </row>
     <row r="6">
@@ -1996,7 +1996,7 @@
         <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>77.71415804389517</v>
+        <v>77.71415804389518</v>
       </c>
     </row>
     <row r="10">
@@ -2007,7 +2007,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>77.69570955930803</v>
+        <v>77.69570955930804</v>
       </c>
     </row>
     <row r="11">
@@ -2051,7 +2051,7 @@
         <v>110</v>
       </c>
       <c r="C14" t="n">
-        <v>85.86449486181279</v>
+        <v>85.86449486181277</v>
       </c>
     </row>
     <row r="15">
@@ -2084,7 +2084,7 @@
         <v>90</v>
       </c>
       <c r="C17" t="n">
-        <v>83.5334297472958</v>
+        <v>83.53342974729578</v>
       </c>
     </row>
     <row r="18">
@@ -2095,7 +2095,7 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>83.53752261949603</v>
+        <v>83.53752261949606</v>
       </c>
     </row>
     <row r="19">
@@ -2106,7 +2106,7 @@
         <v>90</v>
       </c>
       <c r="C19" t="n">
-        <v>83.21896062299719</v>
+        <v>83.2189606229972</v>
       </c>
     </row>
     <row r="20">
@@ -2128,7 +2128,7 @@
         <v>30</v>
       </c>
       <c r="C21" t="n">
-        <v>40.50903357825488</v>
+        <v>40.50903357825487</v>
       </c>
     </row>
     <row r="22">
@@ -2150,7 +2150,7 @@
         <v>50</v>
       </c>
       <c r="C23" t="n">
-        <v>59.19251032195404</v>
+        <v>59.19251032195403</v>
       </c>
     </row>
     <row r="24">
@@ -2161,7 +2161,7 @@
         <v>30</v>
       </c>
       <c r="C24" t="n">
-        <v>39.14283676219369</v>
+        <v>39.1428367621937</v>
       </c>
     </row>
     <row r="25">
@@ -2172,7 +2172,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>58.09640095917622</v>
+        <v>58.09640095917624</v>
       </c>
     </row>
     <row r="26">
@@ -2194,7 +2194,7 @@
         <v>110</v>
       </c>
       <c r="C27" t="n">
-        <v>84.46808909385726</v>
+        <v>84.46808909385727</v>
       </c>
     </row>
     <row r="28">
@@ -2216,7 +2216,7 @@
         <v>110</v>
       </c>
       <c r="C29" t="n">
-        <v>84.36952520178278</v>
+        <v>84.36952520178279</v>
       </c>
     </row>
     <row r="30">
@@ -2238,7 +2238,7 @@
         <v>100</v>
       </c>
       <c r="C31" t="n">
-        <v>83.94897988039341</v>
+        <v>83.94897988039342</v>
       </c>
     </row>
     <row r="32">
@@ -2249,7 +2249,7 @@
         <v>100</v>
       </c>
       <c r="C32" t="n">
-        <v>84.16199967493081</v>
+        <v>84.16199967493083</v>
       </c>
     </row>
     <row r="33">
@@ -2271,7 +2271,7 @@
         <v>90</v>
       </c>
       <c r="C34" t="n">
-        <v>80.66965563443522</v>
+        <v>80.6696556344352</v>
       </c>
     </row>
     <row r="35">
@@ -2293,7 +2293,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="n">
-        <v>71.46701152805296</v>
+        <v>71.46701152805295</v>
       </c>
     </row>
     <row r="37">
@@ -2315,7 +2315,7 @@
         <v>50</v>
       </c>
       <c r="C38" t="n">
-        <v>55.82895092659501</v>
+        <v>55.82895092659504</v>
       </c>
     </row>
     <row r="39">
@@ -2326,7 +2326,7 @@
         <v>110</v>
       </c>
       <c r="C39" t="n">
-        <v>82.08142403989854</v>
+        <v>82.08142403989855</v>
       </c>
     </row>
     <row r="40">
@@ -2337,7 +2337,7 @@
         <v>110</v>
       </c>
       <c r="C40" t="n">
-        <v>82.04752648045647</v>
+        <v>82.04752648045648</v>
       </c>
     </row>
     <row r="41">
@@ -2348,7 +2348,7 @@
         <v>100</v>
       </c>
       <c r="C41" t="n">
-        <v>81.39474708620664</v>
+        <v>81.39474708620665</v>
       </c>
     </row>
     <row r="42">
@@ -2370,7 +2370,7 @@
         <v>90</v>
       </c>
       <c r="C43" t="n">
-        <v>78.74138865155787</v>
+        <v>78.74138865155786</v>
       </c>
     </row>
     <row r="44">
@@ -2381,7 +2381,7 @@
         <v>90</v>
       </c>
       <c r="C44" t="n">
-        <v>78.73314738781856</v>
+        <v>78.73314738781852</v>
       </c>
     </row>
     <row r="45">
@@ -2392,7 +2392,7 @@
         <v>30</v>
       </c>
       <c r="C45" t="n">
-        <v>35.97784137708924</v>
+        <v>35.97784137708925</v>
       </c>
     </row>
     <row r="46">
@@ -2436,7 +2436,7 @@
         <v>50</v>
       </c>
       <c r="C49" t="n">
-        <v>53.30495415093972</v>
+        <v>53.30495415093973</v>
       </c>
     </row>
     <row r="50">
@@ -2447,7 +2447,7 @@
         <v>50</v>
       </c>
       <c r="C50" t="n">
-        <v>53.24802396573912</v>
+        <v>53.2480239657391</v>
       </c>
     </row>
     <row r="51">
@@ -2458,7 +2458,7 @@
         <v>110</v>
       </c>
       <c r="C51" t="n">
-        <v>80.18058245827233</v>
+        <v>80.18058245827234</v>
       </c>
     </row>
     <row r="52">
@@ -2480,7 +2480,7 @@
         <v>110</v>
       </c>
       <c r="C53" t="n">
-        <v>80.4831812095473</v>
+        <v>80.48318120954728</v>
       </c>
     </row>
     <row r="54">
@@ -2491,7 +2491,7 @@
         <v>100</v>
       </c>
       <c r="C54" t="n">
-        <v>78.21669381977901</v>
+        <v>78.21669381977905</v>
       </c>
     </row>
     <row r="55">
@@ -2502,7 +2502,7 @@
         <v>100</v>
       </c>
       <c r="C55" t="n">
-        <v>79.130205461584</v>
+        <v>79.13020546158401</v>
       </c>
     </row>
     <row r="56">
@@ -2524,7 +2524,7 @@
         <v>90</v>
       </c>
       <c r="C57" t="n">
-        <v>74.97702479817868</v>
+        <v>74.97702479817869</v>
       </c>
     </row>
     <row r="58">
@@ -2557,7 +2557,7 @@
         <v>30</v>
       </c>
       <c r="C60" t="n">
-        <v>34.17120834657037</v>
+        <v>34.17120834657039</v>
       </c>
     </row>
     <row r="61">
@@ -2568,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="C61" t="n">
-        <v>65.78815601751637</v>
+        <v>65.78815601751636</v>
       </c>
     </row>
     <row r="62">
@@ -2579,7 +2579,7 @@
         <v>30</v>
       </c>
       <c r="C62" t="n">
-        <v>34.1046151541298</v>
+        <v>34.10461515412981</v>
       </c>
     </row>
     <row r="63">
@@ -2590,7 +2590,7 @@
         <v>70</v>
       </c>
       <c r="C63" t="n">
-        <v>65.69432727432593</v>
+        <v>65.69432727432594</v>
       </c>
     </row>
     <row r="64">
@@ -2612,7 +2612,7 @@
         <v>110</v>
       </c>
       <c r="C65" t="n">
-        <v>79.58927184402705</v>
+        <v>79.58927184402708</v>
       </c>
     </row>
     <row r="66">
@@ -2623,7 +2623,7 @@
         <v>50</v>
       </c>
       <c r="C66" t="n">
-        <v>50.91527557753373</v>
+        <v>50.91527557753371</v>
       </c>
     </row>
     <row r="67">
@@ -2645,7 +2645,7 @@
         <v>50</v>
       </c>
       <c r="C68" t="n">
-        <v>50.66989937892256</v>
+        <v>50.66989937892258</v>
       </c>
     </row>
     <row r="69">
@@ -2656,7 +2656,7 @@
         <v>100</v>
       </c>
       <c r="C69" t="n">
-        <v>75.79828203839129</v>
+        <v>75.79828203839131</v>
       </c>
     </row>
     <row r="70">
@@ -2689,7 +2689,7 @@
         <v>90</v>
       </c>
       <c r="C72" t="n">
-        <v>72.98666563762727</v>
+        <v>72.98666563762724</v>
       </c>
     </row>
     <row r="73">
@@ -2700,7 +2700,7 @@
         <v>90</v>
       </c>
       <c r="C73" t="n">
-        <v>72.93490384262768</v>
+        <v>72.9349038426277</v>
       </c>
     </row>
     <row r="74">
@@ -2733,7 +2733,7 @@
         <v>30</v>
       </c>
       <c r="C76" t="n">
-        <v>32.02547337800175</v>
+        <v>32.02547337800176</v>
       </c>
     </row>
     <row r="77">
@@ -2755,7 +2755,7 @@
         <v>30</v>
       </c>
       <c r="C78" t="n">
-        <v>32.22784086058083</v>
+        <v>32.22784086058086</v>
       </c>
     </row>
     <row r="79">
@@ -2777,7 +2777,7 @@
         <v>50</v>
       </c>
       <c r="C80" t="n">
-        <v>48.33747996471524</v>
+        <v>48.33747996471525</v>
       </c>
     </row>
     <row r="81">
@@ -2788,7 +2788,7 @@
         <v>50</v>
       </c>
       <c r="C81" t="n">
-        <v>48.25987218664558</v>
+        <v>48.25987218664559</v>
       </c>
     </row>
     <row r="82">
@@ -2799,7 +2799,7 @@
         <v>110</v>
       </c>
       <c r="C82" t="n">
-        <v>75.42647972373051</v>
+        <v>75.42647972373054</v>
       </c>
     </row>
     <row r="83">
@@ -2810,7 +2810,7 @@
         <v>110</v>
       </c>
       <c r="C83" t="n">
-        <v>76.00080175862865</v>
+        <v>76.00080175862864</v>
       </c>
     </row>
     <row r="84">
@@ -2843,7 +2843,7 @@
         <v>100</v>
       </c>
       <c r="C86" t="n">
-        <v>72.91544350998512</v>
+        <v>72.91544350998511</v>
       </c>
     </row>
     <row r="87">
@@ -2854,7 +2854,7 @@
         <v>90</v>
       </c>
       <c r="C87" t="n">
-        <v>69.83911551587111</v>
+        <v>69.83911551587113</v>
       </c>
     </row>
     <row r="88">
@@ -2865,7 +2865,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="n">
-        <v>69.7740002811617</v>
+        <v>69.77400028116173</v>
       </c>
     </row>
     <row r="89">
@@ -2876,7 +2876,7 @@
         <v>30</v>
       </c>
       <c r="C89" t="n">
-        <v>30.47378059016826</v>
+        <v>30.47378059016827</v>
       </c>
     </row>
     <row r="90">
@@ -2887,7 +2887,7 @@
         <v>30</v>
       </c>
       <c r="C90" t="n">
-        <v>30.44897009956411</v>
+        <v>30.44897009956412</v>
       </c>
     </row>
     <row r="91">
@@ -2898,7 +2898,7 @@
         <v>70</v>
       </c>
       <c r="C91" t="n">
-        <v>58.67419889348076</v>
+        <v>58.67419889348074</v>
       </c>
     </row>
     <row r="92">
@@ -2920,7 +2920,7 @@
         <v>50</v>
       </c>
       <c r="C93" t="n">
-        <v>44.88179549308946</v>
+        <v>44.88179549308948</v>
       </c>
     </row>
     <row r="94">
@@ -2942,7 +2942,7 @@
         <v>110</v>
       </c>
       <c r="C95" t="n">
-        <v>71.91799025526349</v>
+        <v>71.9179902552635</v>
       </c>
     </row>
     <row r="96">
@@ -2953,7 +2953,7 @@
         <v>50</v>
       </c>
       <c r="C96" t="n">
-        <v>44.88747445090792</v>
+        <v>44.88747445090791</v>
       </c>
     </row>
     <row r="97">
@@ -2964,7 +2964,7 @@
         <v>50</v>
       </c>
       <c r="C97" t="n">
-        <v>44.88685149336632</v>
+        <v>44.88685149336631</v>
       </c>
     </row>
     <row r="98">
@@ -2975,7 +2975,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="n">
-        <v>68.75662438391234</v>
+        <v>68.75662438391235</v>
       </c>
     </row>
     <row r="99">
@@ -2986,7 +2986,7 @@
         <v>100</v>
       </c>
       <c r="C99" t="n">
-        <v>68.86816732128658</v>
+        <v>68.86816732128656</v>
       </c>
     </row>
     <row r="100">
@@ -2997,7 +2997,7 @@
         <v>30</v>
       </c>
       <c r="C100" t="n">
-        <v>29.14681352124826</v>
+        <v>29.14681352124827</v>
       </c>
     </row>
     <row r="101">
@@ -3030,7 +3030,7 @@
         <v>30</v>
       </c>
       <c r="C103" t="n">
-        <v>28.81196853338992</v>
+        <v>28.81196853338993</v>
       </c>
     </row>
     <row r="104">
@@ -3107,7 +3107,7 @@
         <v>50</v>
       </c>
       <c r="C110" t="n">
-        <v>42.3963056191545</v>
+        <v>42.39630561915451</v>
       </c>
     </row>
     <row r="111">
@@ -3118,7 +3118,7 @@
         <v>30</v>
       </c>
       <c r="C111" t="n">
-        <v>27.84026769752869</v>
+        <v>27.84026769752868</v>
       </c>
     </row>
     <row r="112">
@@ -3184,7 +3184,7 @@
         <v>90</v>
       </c>
       <c r="C117" t="n">
-        <v>61.60583411459603</v>
+        <v>61.60583411459604</v>
       </c>
     </row>
     <row r="118">
@@ -3206,7 +3206,7 @@
         <v>90</v>
       </c>
       <c r="C119" t="n">
-        <v>61.22077596975796</v>
+        <v>61.22077596975797</v>
       </c>
     </row>
     <row r="120">
@@ -3261,7 +3261,7 @@
         <v>50</v>
       </c>
       <c r="C124" t="n">
-        <v>40.50269326356608</v>
+        <v>40.50269326356607</v>
       </c>
     </row>
     <row r="125">
@@ -3283,7 +3283,7 @@
         <v>30</v>
       </c>
       <c r="C126" t="n">
-        <v>26.73407984646858</v>
+        <v>26.73407984646859</v>
       </c>
     </row>
     <row r="127">

</xml_diff>